<commit_message>
refine the third part
</commit_message>
<xml_diff>
--- a/实验配置.xlsx
+++ b/实验配置.xlsx
@@ -9,7 +9,8 @@
   <sheets>
     <sheet name="数据库" sheetId="1" r:id="rId1"/>
     <sheet name="实验配置" sheetId="2" r:id="rId2"/>
-    <sheet name="评价方法" sheetId="3" r:id="rId3"/>
+    <sheet name="初始Default Box设置" sheetId="4" r:id="rId3"/>
+    <sheet name="评价方法" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="89">
   <si>
     <t>挑选的样本数</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -152,10 +153,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Linux 16.04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GeForce GTX 1080</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -169,10 +166,6 @@
   </si>
   <si>
     <t>负</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>样本类别</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -198,6 +191,205 @@
   <si>
     <t>GroundTruth
 (nGt = TP + FN)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conv4_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fc7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conv6_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conv7_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conv8_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conv9_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10~20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20-37</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37-54</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>54-71</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>71-88</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>88-100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[1, 4, 8]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[1, 4, 8]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实际要考虑k和1/k两种，这里为了简化，只写出k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Default Box的尺度sk设置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第1层大小: 10~20
+第2层至第6层大小: 20~100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>尺度(%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>长宽比</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Default Box设置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图像数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单词数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>训练集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>标注信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ICDAR2013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原始数据集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试/验证集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挑选为训练库的图像数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COCO-Text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCUT_FORU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>标注内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单词</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位置，内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单词，字符</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单词，字符，分割</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总数据集
+(有标注）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本文训练库（cocoICDAR13SCUT）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单词</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>标注等级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位置，文字内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位置，文字内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位置，文字内容，易读性，类别，语言，编码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总数据集(有标注）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>内核版本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ubuntu 16.04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.4.0-71-generic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Detection
+GroundTruth</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -205,7 +397,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +412,40 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="黑体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000066"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -229,7 +455,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -252,11 +478,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalDown="1">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -264,15 +544,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -280,6 +607,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF000066"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -554,26 +886,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M6"/>
+  <dimension ref="B2:S26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M6"/>
+    <sheetView topLeftCell="G16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q21" sqref="L20:S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="7.125" customWidth="1"/>
+    <col min="4" max="4" width="7.5" customWidth="1"/>
+    <col min="5" max="5" width="7.125" customWidth="1"/>
     <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.75" customWidth="1"/>
-    <col min="12" max="12" width="28.625" customWidth="1"/>
-    <col min="13" max="13" width="18.125" customWidth="1"/>
+    <col min="7" max="7" width="7.125" customWidth="1"/>
+    <col min="8" max="8" width="7.5" customWidth="1"/>
+    <col min="9" max="9" width="12.875" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="15.125" customWidth="1"/>
+    <col min="12" max="12" width="11.75" customWidth="1"/>
+    <col min="13" max="13" width="7.125" customWidth="1"/>
+    <col min="14" max="14" width="7.5" customWidth="1"/>
+    <col min="15" max="17" width="7.125" customWidth="1"/>
+    <col min="18" max="18" width="10" customWidth="1"/>
+    <col min="19" max="19" width="21.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:14" ht="57" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -587,29 +926,30 @@
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="185.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:14" ht="185.25" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
@@ -625,30 +965,31 @@
       <c r="F3" s="1">
         <v>63686</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1">
         <v>118309</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>27550</v>
       </c>
-      <c r="I3" s="1">
-        <f>SUM(G3:H3)</f>
+      <c r="J3" s="1">
+        <f>SUM(H3:I3)</f>
         <v>145859</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>6</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="57" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:14" ht="57" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
@@ -664,25 +1005,26 @@
       <c r="F4" s="1">
         <v>462</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1">
         <v>849</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>1095</v>
       </c>
-      <c r="I4" s="1">
-        <f>SUM(G4:H4)</f>
+      <c r="J4" s="1">
+        <f>SUM(H4:I4)</f>
         <v>1944</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="2:13" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="2:14" ht="71.25" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
@@ -698,30 +1040,31 @@
       <c r="F5" s="1">
         <v>1715</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
         <v>3840</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>1581</v>
       </c>
-      <c r="I5" s="1">
-        <f>SUM(G5:H5)</f>
+      <c r="J5" s="1">
+        <f>SUM(H5:I5)</f>
         <v>5421</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -738,8 +1081,368 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B11" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="19"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B12" s="19"/>
+      <c r="C12" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B13" s="19"/>
+      <c r="C13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="20"/>
+      <c r="J13" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B14" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="5">
+        <v>229</v>
+      </c>
+      <c r="D14" s="5">
+        <v>849</v>
+      </c>
+      <c r="E14" s="5">
+        <v>233</v>
+      </c>
+      <c r="F14" s="5">
+        <v>462</v>
+      </c>
+      <c r="G14" s="5">
+        <f>SUM(C14+E14)</f>
+        <v>462</v>
+      </c>
+      <c r="H14" s="5">
+        <f>SUM(D14+F14)</f>
+        <v>1311</v>
+      </c>
+      <c r="I14" s="5">
+        <v>229</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="57" x14ac:dyDescent="0.2">
+      <c r="B15" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="5">
+        <v>43686</v>
+      </c>
+      <c r="D15" s="5">
+        <v>118309</v>
+      </c>
+      <c r="E15" s="5">
+        <v>10000</v>
+      </c>
+      <c r="F15" s="5">
+        <v>27550</v>
+      </c>
+      <c r="G15" s="5">
+        <f t="shared" ref="G15:G16" si="0">SUM(C15+E15)</f>
+        <v>53686</v>
+      </c>
+      <c r="H15" s="5">
+        <f t="shared" ref="H15:H16" si="1">SUM(D15+F15)</f>
+        <v>145859</v>
+      </c>
+      <c r="I15" s="5">
+        <v>1790</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1200</v>
+      </c>
+      <c r="D16" s="5">
+        <v>3840</v>
+      </c>
+      <c r="E16" s="5">
+        <v>515</v>
+      </c>
+      <c r="F16" s="5">
+        <v>1581</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" si="0"/>
+        <v>1715</v>
+      </c>
+      <c r="H16" s="5">
+        <f t="shared" si="1"/>
+        <v>5421</v>
+      </c>
+      <c r="I16" s="5">
+        <v>1560</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B17" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="18">
+        <f>SUM(I14:I16)</f>
+        <v>3579</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="L20" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="M20" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="L21" s="19"/>
+      <c r="M21" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="R21" s="20"/>
+      <c r="S21" s="20"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="L22" s="19"/>
+      <c r="M22" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="N22" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="O22" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="P22" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q22" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="R22" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="S22" s="20"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="L23" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="M23" s="5">
+        <v>229</v>
+      </c>
+      <c r="N23" s="5">
+        <v>849</v>
+      </c>
+      <c r="O23" s="5">
+        <v>233</v>
+      </c>
+      <c r="P23" s="5">
+        <v>462</v>
+      </c>
+      <c r="Q23" s="5">
+        <f>SUM(M23+O23)</f>
+        <v>462</v>
+      </c>
+      <c r="R23" s="5">
+        <f>SUM(N23+P23)</f>
+        <v>1311</v>
+      </c>
+      <c r="S23" s="5">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="L24" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="M24" s="5">
+        <v>43686</v>
+      </c>
+      <c r="N24" s="5">
+        <v>118309</v>
+      </c>
+      <c r="O24" s="5">
+        <v>10000</v>
+      </c>
+      <c r="P24" s="5">
+        <v>27550</v>
+      </c>
+      <c r="Q24" s="5">
+        <f t="shared" ref="Q24:Q25" si="2">SUM(M24+O24)</f>
+        <v>53686</v>
+      </c>
+      <c r="R24" s="5">
+        <f t="shared" ref="R24:R25" si="3">SUM(N24+P24)</f>
+        <v>145859</v>
+      </c>
+      <c r="S24" s="5">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="L25" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="M25" s="5">
+        <v>1200</v>
+      </c>
+      <c r="N25" s="5">
+        <v>3840</v>
+      </c>
+      <c r="O25" s="5">
+        <v>515</v>
+      </c>
+      <c r="P25" s="5">
+        <v>1581</v>
+      </c>
+      <c r="Q25" s="5">
+        <f t="shared" si="2"/>
+        <v>1715</v>
+      </c>
+      <c r="R25" s="5">
+        <f t="shared" si="3"/>
+        <v>5421</v>
+      </c>
+      <c r="S25" s="5">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="L26" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="18">
+        <f>SUM(S23:S25)</f>
+        <v>3579</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="L26:R26"/>
+    <mergeCell ref="L20:L22"/>
+    <mergeCell ref="M20:R20"/>
+    <mergeCell ref="S20:S22"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="J11:K12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="C11:H11"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -748,10 +1451,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C5"/>
+  <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="B2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -760,35 +1463,43 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="3" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -799,63 +1510,182 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E5"/>
+  <dimension ref="C2:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="11.75" customWidth="1"/>
+    <col min="4" max="4" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.125" customWidth="1"/>
+    <col min="6" max="9" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C2" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C3" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="C5" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:J2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14.375" customWidth="1"/>
+    <col min="3" max="3" width="19.375" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
     <col min="5" max="5" width="17.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="3"/>
+      <c r="C2" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="17"/>
+      <c r="C4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="17"/>
+      <c r="C5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="6"/>
-      <c r="C4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="6"/>
-      <c r="C5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>